<commit_message>
Completed Milestone 3: Evaluation and Refinement
</commit_message>
<xml_diff>
--- a/docs/Defect_Tracker Template_v0.1.xlsx
+++ b/docs/Defect_Tracker Template_v0.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d79fe2bc3d7eff9/Desktop/AI-Enabled-Recommendation-Engine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d79fe2bc3d7eff9/Desktop/AI-Enabled-Recommendation-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:101_{A9B59A9A-789B-4A89-A90D-BB9A1B756E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5642DA9E-E007-4437-9D08-5F4065567943}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="13_ncr:101_{A9B59A9A-789B-4A89-A90D-BB9A1B756E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{233783FB-CB1A-4448-8F25-039E1C721FB6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Sl No</t>
   </si>
@@ -111,6 +111,60 @@
   </si>
   <si>
     <t>dataset  size was inconsistent after preprocessing</t>
+  </si>
+  <si>
+    <t>incorrect recommendations henerated for some users</t>
+  </si>
+  <si>
+    <t>Fixed item similarity calculation and recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommendation output verifiad and corrected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate items appearing in recommendation list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applied filering to remove duplicate items </t>
+  </si>
+  <si>
+    <t>Final recommendation list cleand</t>
+  </si>
+  <si>
+    <t>Precision  and recall values not calculated correctly</t>
+  </si>
+  <si>
+    <t>milestone3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrected evaluation metric formulas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Closed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrices validated with sampal test data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model acuracy was low for some test scenarios </t>
+  </si>
+  <si>
+    <t>Improvetuned  recommendation logic and fine-tuned parameters</t>
+  </si>
+  <si>
+    <t>Improved F1  score  after refinement</t>
+  </si>
+  <si>
+    <t>Recommendation model was generating duplicate item suggestions for the same user</t>
+  </si>
+  <si>
+    <t>Added duplicate filtering logic and validated unique recommendation</t>
+  </si>
+  <si>
+    <t>issue resolved and output verified</t>
   </si>
 </sst>
 </file>
@@ -136,38 +190,38 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Aptos"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="56"/>
-      <name val="Aptos"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="56"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Aptos"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Aptos"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="56"/>
-      <name val="Aptos"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -223,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -233,45 +287,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -288,10 +357,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,22 +648,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.54296875" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="42.1796875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="21.81640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="17.54296875" style="10"/>
+    <col min="1" max="1" width="6.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="42.1796875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="21.81640625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="17.54296875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.4">
@@ -649,29 +714,29 @@
       <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="8">
-        <v>46027</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="9">
+        <v>46025</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -684,25 +749,25 @@
       <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="8">
-        <v>46028</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="9">
+        <v>46027</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -719,50 +784,62 @@
       <c r="D4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="9">
         <v>46029</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="48" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8">
-        <v>46031</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="C5" s="6">
+        <v>46040</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="9">
+        <v>46032</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="48" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
@@ -771,217 +848,281 @@
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="C6" s="6">
+        <v>46040</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="9">
+        <v>46035</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.4">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="17">
+        <v>46040</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="9">
+        <v>46037</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.4">
-      <c r="A9" s="14">
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6">
+        <v>46050</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="9">
+        <v>46043</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="64" x14ac:dyDescent="0.4">
+      <c r="A9" s="22">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="17"/>
+      <c r="B9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="17">
+        <v>46050</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="23">
+        <v>46043</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1045,21 +1186,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F50FC49184C87E449886FB52439922C9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85b7e58c3d8889ba0673e7b34a193a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67b99c0-208c-4860-83e0-51466af787c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d43477c1ade21a66d9a75ba2d5aa042" ns2:_="">
     <xsd:import namespace="b67b99c0-208c-4860-83e0-51466af787c4"/>
@@ -1191,24 +1317,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191CB444-B9BF-4C91-94BD-600524521497}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1224,4 +1348,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>